<commit_message>
Added ApiEceptionFilter (globally thru Global.asa) Updated uspCalcTodaysMatchups to fix calc of Opposite RotNum
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Async processing.xlsx
+++ b/BballMVC/_Documentation/Async processing.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E7F0DAB-7F2D-4937-9D1B-28F42BC74D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2A87CA-7D8C-466D-B2C0-9DAF58B27B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31035" yWindow="600" windowWidth="22350" windowHeight="13470" xr2:uid="{EFF91725-B809-48EF-AC47-0E20FA8C8787}"/>
+    <workbookView xWindow="62085" yWindow="1845" windowWidth="22350" windowHeight="13470" activeTab="2" xr2:uid="{EFF91725-B809-48EF-AC47-0E20FA8C8787}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Async" sheetId="1" r:id="rId1"/>
+    <sheet name="Filters" sheetId="2" r:id="rId2"/>
+    <sheet name="Security" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,16 +27,203 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>https://docs.microsoft.com/en-us/dotnet/csharp/programming-guide/concepts/async/</t>
+  </si>
+  <si>
+    <t>Filter Type</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Simple Filter</t>
+  </si>
+  <si>
+    <t>IFilter</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Defines the methods that are used in a filter</t>
+  </si>
+  <si>
+    <t>Action Filter</t>
+  </si>
+  <si>
+    <t>IActionFilter</t>
+  </si>
+  <si>
+    <t>ActionFilterAttribute</t>
+  </si>
+  <si>
+    <t>Used to add extra logic before or after action methods execute.</t>
+  </si>
+  <si>
+    <t>Authentication Filter</t>
+  </si>
+  <si>
+    <t>IAuthenticationFilter</t>
+  </si>
+  <si>
+    <t>Used to force users or clients to be authenticated before action methods execute.</t>
+  </si>
+  <si>
+    <t>Authorization Filter</t>
+  </si>
+  <si>
+    <t>IAuthorizationFilter</t>
+  </si>
+  <si>
+    <t>AuthorizationFilterAttribute</t>
+  </si>
+  <si>
+    <t>Used to restrict access to action methods to specific users or groups.</t>
+  </si>
+  <si>
+    <t>Exception Filter</t>
+  </si>
+  <si>
+    <t>IExceptionFilter</t>
+  </si>
+  <si>
+    <t>ExceptionFilterAttribute</t>
+  </si>
+  <si>
+    <t>Used to handle all unhandled exception in Web API.</t>
+  </si>
+  <si>
+    <t>Override Filter</t>
+  </si>
+  <si>
+    <t>IOverrideFilter</t>
+  </si>
+  <si>
+    <t>Used to customize the behaviour of other filter for individual action method.</t>
+  </si>
+  <si>
+    <t>https://stackify.com/web-api-error-handling/</t>
+  </si>
+  <si>
+    <t>Web API Error Handling: How To Make Debugging Easier</t>
+  </si>
+  <si>
+    <t>Http error codes</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/dotnet/api/system.net.httpstatuscode?view=netcore-3.1#examples</t>
+  </si>
+  <si>
+    <t>2. Create a GlobalExceptionHandler</t>
+  </si>
+  <si>
+    <t>First off, why would we want to use a GlobalErrorHandler over an ExceptionFilterAttribute? Well, there are some exceptions that our filters will not catch.</t>
+  </si>
+  <si>
+    <t>From the ASP.NET site, there are errors that will not be caught by our filters above. This includes exceptions thrown:</t>
+  </si>
+  <si>
+    <t>1. From controller constructors</t>
+  </si>
+  <si>
+    <t>2. From message handlers</t>
+  </si>
+  <si>
+    <t>3. During routing</t>
+  </si>
+  <si>
+    <t>4. During response content serialization</t>
+  </si>
+  <si>
+    <t>And since we want to be covered in these scenarios as well, let’s add our GlobalExceptionHandler.</t>
+  </si>
+  <si>
+    <t>ExecuteAsync</t>
+  </si>
+  <si>
+    <r>
+      <t>An </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>AJAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> call can be secured the same way any HTTP request can be secured. First of all, use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> as opposed to GET to hide any sensitive parameters from the URL. Secondly, cross check all your requests for CSRF(Cross-Site Request Forgery) by using a CSRF token.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF70757A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.quora.com/How-do-I-make-AJAX-calls-secure</t>
+  </si>
+  <si>
+    <t>An AJAX call can be secured the same way any HTTP request can be secured. First of all, use POST as opposed to GET to hide any sensitive parameters from the URL. Secondly, cross check all your requests for CSRF(Cross-Site Request Forgery) by using a CSRF token. You create this token on the server and serve it as metadata to the page where your JavaSript is loaded. Then send all your AJAX calls together with this token, then on the server side, ensure the tokens match before processing any request.</t>
+  </si>
+  <si>
+    <t>The other thing would be to run the entire URL text and request parameters through a XSS(Cross-Site Scripting) filter before actually sending the request to the server. This filter should remove all JavaSript-like text from the URL text and request parameters i.e characters like “{”, “}”, “(”, “)” and “;” are all required by JavaSript. This ensures no arbitrary JavasSript gets uploaded to the server. Or gets executed before or after the AJAX call.</t>
+  </si>
+  <si>
+    <t>To make it easier, you can use the same filter to filter out any SQL from the URL text and request parameters. This ensures that all SQL injection attacks have been prevented. Comparative characters like “=”, “&lt;” and “&gt;” together with terms like “SELECT” and “FROM” must be removed from all the parameters and from the URL itself to secure your request from SQL injection.</t>
+  </si>
+  <si>
+    <t>Finally, you should run your AJAX calls through an SSL or TLS encrypted HTTPS connection as opposed to normal plain-text HTTP.</t>
+  </si>
+  <si>
+    <t>There is however much more you can do to secure your AJAX calls depending on the nature of your web server, your application client i.e. whether it is browser-based or mobile, your application architecture and other factors. But the above should give pretty good basic security.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,16 +239,106 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF414141"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF414141"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF70757A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF282829"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF63A9E0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -67,14 +346,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFDFDF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFDFDF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFDFDF"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDFDFDF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDFDFDF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDFDFDF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDFDFDF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -219,6 +563,187 @@
         <a:xfrm>
           <a:off x="0" y="4000500"/>
           <a:ext cx="5639587" cy="4182059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7668695</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>804</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F65A69-101E-46A0-B8CD-7A9C3D5E09F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11077575" y="1657350"/>
+          <a:ext cx="7668695" cy="5763429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7868748</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>10351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7718E4BB-09B9-4DBD-9618-F08DEA5B4DB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11077575" y="7610475"/>
+          <a:ext cx="7868748" cy="5915851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1819275</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114795</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E89464-6337-4CA1-93F6-93B16B681263}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3038475"/>
+          <a:ext cx="4848225" cy="3543795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1838582</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>181160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D85BC728-D57B-4747-BED0-EC8FFF966578}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5057775" y="3228975"/>
+          <a:ext cx="1838582" cy="1324160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -529,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798E011B-7ACE-463B-BA45-42881BE729FD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,4 +1076,254 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F70FD02-69A7-4E42-B217-49110FA20972}">
+  <dimension ref="A1:E82"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.28515625" customWidth="1"/>
+    <col min="5" max="5" width="118.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="6" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="E72" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="E73" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E75" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E76" s="11"/>
+    </row>
+    <row r="77" spans="5:5" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="E77" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="5:5" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="E78" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="5:5" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="E79" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="5:5" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="E80" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="82" spans="5:5" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="E82" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{DA61AD29-FD61-4913-8B35-E7A85F7F5A27}"/>
+    <hyperlink ref="A13" r:id="rId2" location="examples" display="https://docs.microsoft.com/en-us/dotnet/api/system.net.httpstatuscode?view=netcore-3.1 - examples" xr:uid="{FA615676-93F9-4A1B-8A35-BA6DF4AB0239}"/>
+    <hyperlink ref="E75" r:id="rId3" display="https://docs.microsoft.com/en-us/aspnet/web-api/overview/error-handling/web-api-global-error-handling" xr:uid="{F1C770FB-9907-42A7-B372-1F7C5C24576E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098F4D53-75C0-476B-972D-01B64A77B11A}">
+  <dimension ref="B2:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="76.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="62.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="99" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="33" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="66" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{A1D49D1B-5266-48E1-AA87-2828F5515805}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Started on Daily / Lg stats display Created BballPROD on local
</commit_message>
<xml_diff>
--- a/BballMVC/_Documentation/Async processing.xlsx
+++ b/BballMVC/_Documentation/Async processing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\wwwroot\Test\mrroot123\mrroot123\BballMVCproject\BballMVC\_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2A87CA-7D8C-466D-B2C0-9DAF58B27B23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4616F8C4-FA73-47C3-87B7-A35C895DBD63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62085" yWindow="1845" windowWidth="22350" windowHeight="13470" activeTab="2" xr2:uid="{EFF91725-B809-48EF-AC47-0E20FA8C8787}"/>
+    <workbookView xWindow="29955" yWindow="975" windowWidth="27045" windowHeight="14280" activeTab="1" xr2:uid="{EFF91725-B809-48EF-AC47-0E20FA8C8787}"/>
   </bookViews>
   <sheets>
     <sheet name="Async" sheetId="1" r:id="rId1"/>
@@ -1054,9 +1054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798E011B-7ACE-463B-BA45-42881BE729FD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1082,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F70FD02-69A7-4E42-B217-49110FA20972}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098F4D53-75C0-476B-972D-01B64A77B11A}">
   <dimension ref="B2:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>